<commit_message>
testing phase 1 complete
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cameronclark/Documents/UCT/EEE4022S/EEE4022S_Salinity_JCP24-03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6212C898-FDAB-9F49-9428-A3BB9833A235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB37FB3C-8F50-F944-AEC1-D61D69C15F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{CC746ED0-B61A-5B42-A9B2-4A328CF3FB68}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{CC746ED0-B61A-5B42-A9B2-4A328CF3FB68}"/>
   </bookViews>
   <sheets>
     <sheet name="DAC Range" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Calib measuring range" sheetId="4" r:id="rId3"/>
     <sheet name="Resistance Measuring accuracy" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>VDD</t>
   </si>
@@ -88,13 +88,40 @@
   <si>
     <t>ratio</t>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Multimeter</t>
+  </si>
+  <si>
+    <t>M Corrected</t>
+  </si>
+  <si>
+    <t>S Corrected +</t>
+  </si>
+  <si>
+    <t>S Corrected -</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -127,7 +154,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1814,6 +1841,871 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Resistance Measuring accuracy'!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Resistance Measuring accuracy'!$B$5:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.0000000000000018E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.42</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.8499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.84</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.59</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.72</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.49</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Resistance Measuring accuracy'!$C$5:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.09</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.4800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.35</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.96</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.52</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.09</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.39</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F1D0-9148-BD88-29EBC99E1309}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="10528176"/>
+        <c:axId val="37586032"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="10528176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="37586032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="37586032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="10528176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Resistance Measuring accuracy'!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S Corrected +</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Resistance Measuring accuracy'!$B$5:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.0000000000000018E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.42</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.8499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.84</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.59</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.72</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.49</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Resistance Measuring accuracy'!$E$5:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>3.378597614411339E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0162370302966457</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.212794733304476</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5310634700832244</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.84025235761367</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2405723198506635</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6778774542246904</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.4039357977161835</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.851684149196243</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.8656515951989912</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.5896460834911528</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.7399529687795008</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.4940472701302001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.2102792923462218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.8887409837136708</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EC65-D145-A9F0-CA4A88F97CD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="85199696"/>
+        <c:axId val="1805885935"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="85199696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1805885935"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1805885935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="85199696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1934,6 +2826,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2967,6 +3939,1038 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3592,6 +5596,83 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>412750</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>96838</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>49069</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>11402</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D262D25-F728-96D9-672F-28D509D57B68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>351415</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>31895</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>810347</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>148504</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16EF5966-1784-5CF2-3476-74338C157B1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3917,10 +5998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D87686-F149-5F41-9359-A57699094329}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A9" zoomScale="166" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4363,18 +6444,41 @@
         <v>3.8323</v>
       </c>
     </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="str">
+        <f>SUBSTITUTE(_xlfn.TEXTJOIN(" ",TRUE,B5:B21), ",",".")</f>
+        <v>0 0.206451612903226 0.412903225806452 0.619354838709677 0.825806451612903 1.03225806451613 1.23870967741935 1.44516129032258 1.65161290322581 1.85806451612903 2.06451612903226 2.27096774193548 2.47741935483871 2.68387096774194 2.89032258064516 3.09677419354839 3.3</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" ref="C26:F26" si="3">SUBSTITUTE(_xlfn.TEXTJOIN(" ",TRUE,C5:C21), ",",".")</f>
+        <v>0.00029 0.05771 0.08159 0.1104 0.14257 0.17767 0.21611 0.25702 0.29951 0.3399 0.38418 0.42398 0.47831 0.8307 3.3212 3.3161 3.318</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="3"/>
+        <v>0.00384 0.20963 0.42009 0.6297 0.8366 1.0469 1.2543 1.462 1.6696 1.8732 2.0801 2.287 2.4899 2.6869 2.8172 2.8217 2.8304</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="3"/>
+        <v>0.00029 0.8202 1.0443 1.2606 1.4713 1.6842 1.8941 2.0981 2.307 2.5125 2.7173 2.9261 3.131 3.2658 3.262 3.252 3.2683</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="3"/>
+        <v>0.00002 0.20509 0.41189 0.6178 0.8227 1.0291 1.2318 1.4325 1.6364 1.8371 2.0325 2.2334 2.4415 2.5491 2.5788 2.579 2.5854</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F176E8-BFB6-5F43-87CF-1E9C60FC2534}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="144" workbookViewId="0">
-      <selection activeCell="E4" activeCellId="1" sqref="C4:C18 E4:E18"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4692,8 +6796,19 @@
         <v>2.6609523809523807</v>
       </c>
     </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C21" t="str">
+        <f>SUBSTITUTE(_xlfn.TEXTJOIN(" ",TRUE,C5:C18), ",",".")</f>
+        <v>0.00299 0.20852 0.41849 0.6282 0.8363 1.0419 1.2487 1.4556 1.6649 1.8689 2.0821 2.2859 2.4966 2.6888</v>
+      </c>
+      <c r="E21" t="str">
+        <f>SUBSTITUTE(_xlfn.TEXTJOIN(" ",TRUE,E5:E18), ",",".")</f>
+        <v>0.00483516483516484 0.20952380952381 0.425494505494506 0.626153846153846 0.817142857142857 1.05648351648352 1.26117216117216 1.42315018315018 1.66168498168498 1.88087912087912 2.05575091575092 2.27172161172161 2.45465201465201 2.66095238095238</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -4702,8 +6817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C106622-CFC1-C54B-A24C-C82EC2B9AA63}">
   <dimension ref="A3:D17"/>
   <sheetViews>
-    <sheetView zoomScale="206" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A2" zoomScale="206" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4755,7 +6870,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <f t="shared" ref="A6:A17" si="1">A5+64</f>
+        <f t="shared" ref="A6:A16" si="1">A5+64</f>
         <v>128</v>
       </c>
       <c r="B6">
@@ -4942,20 +7057,431 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D2C5D3-431B-3745-96C5-77D0D99F8462}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView zoomScale="176" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="176" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>-8.8999999999999999E-3</v>
+      </c>
+      <c r="E2">
+        <v>0.93559999999999999</v>
+      </c>
+      <c r="F2">
+        <v>1.0084</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f>0.26</f>
+        <v>0.26</v>
+      </c>
+      <c r="B5">
+        <f>A5-$A$3</f>
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="C5">
+        <v>1.04</v>
+      </c>
+      <c r="D5">
+        <v>1.03</v>
+      </c>
+      <c r="E5">
+        <f>(-$E$2+SQRT($E$2*$E$2-4*$D$2*($F$2-$C5)))/(2*$D$2)</f>
+        <v>3.378597614411339E-2</v>
+      </c>
+      <c r="F5">
+        <f>(-$E$2-SQRT($E$2*$E$2-4*$D$2*($F$2-$C5)))/(2*$D$2)</f>
+        <v>105.08980952947387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1.24</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ref="B6:B19" si="0">A6-$A$3</f>
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1.95</v>
+      </c>
+      <c r="D6">
+        <v>1.94</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:F19" si="1">(-$E$2+SQRT($E$2*$E$2-4*$D$2*($F$2-$C6)))/(2*$D$2)</f>
+        <v>1.0162370302966457</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F19" si="2">(-$E$2-SQRT($E$2*$E$2-4*$D$2*($F$2-$C6)))/(2*$D$2)</f>
+        <v>104.10735847532133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1.45</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>1.21</v>
+      </c>
+      <c r="C7">
+        <v>2.13</v>
+      </c>
+      <c r="D7">
+        <v>2.11</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>1.212794733304476</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>103.91080077231349</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1.76</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>1.52</v>
+      </c>
+      <c r="C8">
+        <v>2.42</v>
+      </c>
+      <c r="D8">
+        <v>2.4</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>1.5310634700832244</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>103.59253203553475</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2.12</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>1.8800000000000001</v>
+      </c>
+      <c r="C9">
+        <v>2.7</v>
+      </c>
+      <c r="D9">
+        <v>2.69</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>1.84025235761367</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>103.28334314800431</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2.5</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="C10">
+        <v>3.06</v>
+      </c>
+      <c r="D10">
+        <v>3.04</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>2.2405723198506635</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>102.88302318576731</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2.92</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>2.6799999999999997</v>
+      </c>
+      <c r="C11">
+        <v>3.45</v>
+      </c>
+      <c r="D11">
+        <v>3.44</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>2.6778774542246904</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>102.44571805139329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>3.66</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>3.42</v>
+      </c>
+      <c r="C12">
+        <v>4.09</v>
+      </c>
+      <c r="D12">
+        <v>4.08</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>3.4039357977161835</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>101.7196597079018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>4.09</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>3.8499999999999996</v>
+      </c>
+      <c r="C13">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="D13">
+        <v>4.47</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>3.851684149196243</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>101.27191135642174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>5.08</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>4.84</v>
+      </c>
+      <c r="C14">
+        <v>5.35</v>
+      </c>
+      <c r="D14">
+        <v>5.35</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>4.8656515951989912</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>100.25794391041899</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>5.83</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>5.59</v>
+      </c>
+      <c r="C15">
+        <v>5.96</v>
+      </c>
+      <c r="D15">
+        <v>5.96</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>5.5896460834911528</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>99.533949422126824</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>6.96</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>6.72</v>
+      </c>
+      <c r="C16">
+        <v>6.91</v>
+      </c>
+      <c r="D16">
+        <v>6.91</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>6.7399529687795008</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>98.383642536838479</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>7.73</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>7.49</v>
+      </c>
+      <c r="C17">
+        <v>7.52</v>
+      </c>
+      <c r="D17">
+        <v>7.52</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>7.4940472701302001</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>97.629548235487775</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>8.44</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C18">
+        <v>8.09</v>
+      </c>
+      <c r="D18">
+        <v>8.1</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>8.2102792923462218</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>96.913316213271756</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>10.14</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>9.9</v>
+      </c>
+      <c r="C19">
+        <v>9.39</v>
+      </c>
+      <c r="D19">
+        <v>9.4</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>9.8887409837136708</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>95.23485452190431</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="str">
+        <f>SUBSTITUTE(_xlfn.TEXTJOIN(" ",TRUE,A5:A19), ",",".")</f>
+        <v>0.26 1.24 1.45 1.76 2.12 2.5 2.92 3.66 4.09 5.08 5.83 6.96 7.73 8.44 10.14</v>
+      </c>
+      <c r="B22" t="str">
+        <f>SUBSTITUTE(_xlfn.TEXTJOIN(" ",TRUE,B5:B19), ",",".")</f>
+        <v>0.02 1 1.21 1.52 1.88 2.26 2.68 3.42 3.85 4.84 5.59 6.72 7.49 8.2 9.9</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" ref="C22:E22" si="3">SUBSTITUTE(_xlfn.TEXTJOIN(" ",TRUE,C5:C19), ",",".")</f>
+        <v>1.04 1.95 2.13 2.42 2.7 3.06 3.45 4.09 4.48 5.35 5.96 6.91 7.52 8.09 9.39</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="3"/>
+        <v>1.03 1.94 2.11 2.4 2.69 3.04 3.44 4.08 4.47 5.35 5.96 6.91 7.52 8.1 9.4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>